<commit_message>
Fix excel template Formatting Problem
</commit_message>
<xml_diff>
--- a/src/main/resources/jxl_template.xlsx
+++ b/src/main/resources/jxl_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brookfield\IdeaProjects\fp\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B74882E-5876-4D06-BF1D-A1112E7D488E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822F2371-D793-48C0-919E-EE2BEC6F7963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -252,18 +252,12 @@
     <t>${product.total}</t>
   </si>
   <si>
-    <t>PHP ${order.total}</t>
-  </si>
-  <si>
     <t>${promo.name}</t>
   </si>
   <si>
     <t>${promo.quantity}</t>
   </si>
   <si>
-    <t>${product.discount.name}</t>
-  </si>
-  <si>
     <t>${trucking.address}</t>
   </si>
   <si>
@@ -295,6 +289,12 @@
   </si>
   <si>
     <t>${generateTime}</t>
+  </si>
+  <si>
+    <t>${product.discount}</t>
+  </si>
+  <si>
+    <t>${order.totalString}</t>
   </si>
 </sst>
 </file>
@@ -807,10 +807,203 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -833,199 +1026,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1556,169 +1556,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="8.25" customHeight="1">
-      <c r="B1" s="89"/>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="91"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="120"/>
+      <c r="D1" s="120"/>
+      <c r="E1" s="120"/>
+      <c r="F1" s="121"/>
     </row>
     <row r="2" spans="1:18" ht="4.5" customHeight="1">
-      <c r="B2" s="92"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="94"/>
+      <c r="B2" s="104"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
+      <c r="H2" s="105"/>
+      <c r="I2" s="105"/>
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="106"/>
       <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="123" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="98"/>
-      <c r="E3" s="98"/>
-      <c r="F3" s="98"/>
-      <c r="G3" s="98"/>
-      <c r="H3" s="98"/>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="99"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="125"/>
       <c r="L3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="95"/>
+      <c r="M3" s="112"/>
       <c r="O3" s="20"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="B4" s="97"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="98"/>
-      <c r="E4" s="98"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="98"/>
-      <c r="H4" s="98"/>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="99"/>
+      <c r="B4" s="123"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
+      <c r="K4" s="125"/>
       <c r="L4" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="95"/>
+      <c r="M4" s="112"/>
       <c r="O4" s="20"/>
     </row>
     <row r="5" spans="1:18" ht="15.75">
-      <c r="B5" s="74"/>
+      <c r="B5" s="110"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="96" t="s">
+      <c r="F5" s="122" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96"/>
-      <c r="J5" s="96"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="95"/>
+      <c r="G5" s="122"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="122"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="122"/>
+      <c r="M5" s="112"/>
       <c r="O5" s="20"/>
     </row>
     <row r="6" spans="1:18" ht="15.75">
-      <c r="B6" s="74"/>
+      <c r="B6" s="110"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="96" t="s">
+      <c r="F6" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="102"/>
+      <c r="G6" s="122"/>
+      <c r="H6" s="122"/>
+      <c r="I6" s="122"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="128"/>
       <c r="L6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="95"/>
+      <c r="M6" s="112"/>
       <c r="O6" s="20"/>
     </row>
     <row r="7" spans="1:18" ht="15.75">
-      <c r="B7" s="74"/>
+      <c r="B7" s="110"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="96" t="s">
+      <c r="F7" s="122" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="122"/>
+      <c r="J7" s="122"/>
+      <c r="K7" s="122"/>
       <c r="L7" s="35" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="95"/>
+        <v>50</v>
+      </c>
+      <c r="M7" s="112"/>
       <c r="O7" s="20"/>
       <c r="P7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="B8" s="74"/>
-      <c r="C8" s="100" t="s">
+      <c r="B8" s="110"/>
+      <c r="C8" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
-      <c r="M8" s="95"/>
+      <c r="D8" s="127"/>
+      <c r="E8" s="127"/>
+      <c r="F8" s="127"/>
+      <c r="G8" s="127"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="127"/>
+      <c r="K8" s="127"/>
+      <c r="L8" s="127"/>
+      <c r="M8" s="112"/>
       <c r="O8" s="20"/>
     </row>
     <row r="9" spans="1:18" ht="16.5" customHeight="1">
-      <c r="B9" s="74"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
-      <c r="M9" s="95"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="127"/>
+      <c r="D9" s="127"/>
+      <c r="E9" s="127"/>
+      <c r="F9" s="127"/>
+      <c r="G9" s="127"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="127"/>
+      <c r="J9" s="127"/>
+      <c r="K9" s="127"/>
+      <c r="L9" s="127"/>
+      <c r="M9" s="112"/>
       <c r="O9" s="20"/>
       <c r="P9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="B10" s="74"/>
-      <c r="C10" s="86" t="s">
+      <c r="B10" s="110"/>
+      <c r="C10" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="71"/>
+      <c r="E10" s="135"/>
+      <c r="F10" s="135"/>
+      <c r="G10" s="135"/>
+      <c r="H10" s="135"/>
+      <c r="I10" s="136"/>
       <c r="J10" s="10"/>
       <c r="K10" s="5" t="s">
         <v>11</v>
@@ -1733,40 +1733,40 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
-      <c r="B11" s="74"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="73"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="137"/>
+      <c r="E11" s="137"/>
+      <c r="F11" s="137"/>
+      <c r="G11" s="137"/>
+      <c r="H11" s="137"/>
+      <c r="I11" s="138"/>
       <c r="J11" s="10"/>
       <c r="K11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="7" t="s">
         <v>49</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="M11" s="19"/>
       <c r="O11" s="20"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
-      <c r="B12" s="74"/>
-      <c r="C12" s="87" t="s">
+      <c r="B12" s="110"/>
+      <c r="C12" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="73" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="83"/>
-      <c r="F12" s="83"/>
-      <c r="G12" s="83"/>
-      <c r="H12" s="83"/>
-      <c r="I12" s="84"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="74"/>
       <c r="J12" s="10"/>
       <c r="K12" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L12" s="7" t="s">
         <v>32</v>
@@ -1775,53 +1775,53 @@
       <c r="O12" s="20"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="B13" s="74"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="103"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="103"/>
-      <c r="G13" s="103"/>
-      <c r="H13" s="103"/>
-      <c r="I13" s="104"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="118"/>
+      <c r="D13" s="129"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
+      <c r="G13" s="129"/>
+      <c r="H13" s="129"/>
+      <c r="I13" s="130"/>
       <c r="J13" s="10"/>
       <c r="K13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M13" s="19"/>
       <c r="O13" s="20"/>
       <c r="P13" s="14"/>
     </row>
     <row r="14" spans="1:18" ht="7.5" customHeight="1">
-      <c r="B14" s="74"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="66"/>
-      <c r="J14" s="66"/>
-      <c r="K14" s="66"/>
-      <c r="L14" s="66"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="111"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
+      <c r="K14" s="111"/>
+      <c r="L14" s="111"/>
       <c r="M14" s="19"/>
       <c r="O14" s="20"/>
       <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:18" ht="15.75">
-      <c r="B15" s="74"/>
+      <c r="B15" s="110"/>
       <c r="C15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="65" t="s">
+      <c r="D15" s="131" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
+      <c r="E15" s="131"/>
+      <c r="F15" s="131"/>
+      <c r="G15" s="131"/>
+      <c r="H15" s="131"/>
       <c r="I15" s="13" t="s">
         <v>4</v>
       </c>
@@ -1839,13 +1839,13 @@
       <c r="R15" s="27"/>
     </row>
     <row r="16" spans="1:18" s="20" customFormat="1" ht="15.75">
-      <c r="B16" s="74"/>
+      <c r="B16" s="110"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="69"/>
+      <c r="D16" s="132"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
+      <c r="G16" s="133"/>
+      <c r="H16" s="134"/>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
@@ -1853,15 +1853,15 @@
       <c r="M16" s="22"/>
     </row>
     <row r="17" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B17" s="74"/>
+      <c r="B17" s="110"/>
       <c r="C17" s="25"/>
-      <c r="D17" s="136" t="s">
+      <c r="D17" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="137"/>
-      <c r="F17" s="137"/>
-      <c r="G17" s="137"/>
-      <c r="H17" s="138"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
@@ -1869,15 +1869,15 @@
       <c r="M17" s="63"/>
     </row>
     <row r="18" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B18" s="74"/>
+      <c r="B18" s="110"/>
       <c r="C18" s="62"/>
-      <c r="D18" s="85" t="s">
+      <c r="D18" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="85"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
       <c r="I18" s="62" t="s">
         <v>36</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>35</v>
       </c>
       <c r="K18" s="62" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="L18" s="61" t="s">
         <v>37</v>
@@ -1893,13 +1893,13 @@
       <c r="M18" s="55"/>
     </row>
     <row r="19" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B19" s="74"/>
+      <c r="B19" s="110"/>
       <c r="C19" s="62"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
+      <c r="D19" s="65"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="65"/>
+      <c r="H19" s="65"/>
       <c r="I19" s="62"/>
       <c r="J19" s="61"/>
       <c r="K19" s="62"/>
@@ -1907,13 +1907,13 @@
       <c r="M19" s="47"/>
     </row>
     <row r="20" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B20" s="74"/>
+      <c r="B20" s="110"/>
       <c r="C20" s="62"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
       <c r="I20" s="62"/>
       <c r="J20" s="61"/>
       <c r="K20" s="62"/>
@@ -1921,13 +1921,13 @@
       <c r="M20" s="56"/>
     </row>
     <row r="21" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B21" s="74"/>
+      <c r="B21" s="110"/>
       <c r="C21" s="62"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="85"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
       <c r="I21" s="62"/>
       <c r="J21" s="61"/>
       <c r="K21" s="62"/>
@@ -1935,13 +1935,13 @@
       <c r="M21" s="63"/>
     </row>
     <row r="22" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B22" s="74"/>
+      <c r="B22" s="110"/>
       <c r="C22" s="62"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="85"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="85"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
       <c r="I22" s="62"/>
       <c r="J22" s="61"/>
       <c r="K22" s="62"/>
@@ -1949,13 +1949,13 @@
       <c r="M22" s="59"/>
     </row>
     <row r="23" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B23" s="74"/>
+      <c r="B23" s="110"/>
       <c r="C23" s="62"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85"/>
+      <c r="D23" s="65"/>
+      <c r="E23" s="65"/>
+      <c r="F23" s="65"/>
+      <c r="G23" s="65"/>
+      <c r="H23" s="65"/>
       <c r="I23" s="62"/>
       <c r="J23" s="61"/>
       <c r="K23" s="62"/>
@@ -1963,13 +1963,13 @@
       <c r="M23" s="53"/>
     </row>
     <row r="24" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B24" s="74"/>
+      <c r="B24" s="110"/>
       <c r="C24" s="62"/>
-      <c r="D24" s="85"/>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="85"/>
+      <c r="D24" s="65"/>
+      <c r="E24" s="65"/>
+      <c r="F24" s="65"/>
+      <c r="G24" s="65"/>
+      <c r="H24" s="65"/>
       <c r="I24" s="62"/>
       <c r="J24" s="61"/>
       <c r="K24" s="62"/>
@@ -1977,13 +1977,13 @@
       <c r="M24" s="52"/>
     </row>
     <row r="25" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B25" s="74"/>
+      <c r="B25" s="110"/>
       <c r="C25" s="62"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
       <c r="I25" s="62"/>
       <c r="J25" s="61"/>
       <c r="K25" s="62"/>
@@ -1991,13 +1991,13 @@
       <c r="M25" s="47"/>
     </row>
     <row r="26" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B26" s="74"/>
+      <c r="B26" s="110"/>
       <c r="C26" s="62"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="85"/>
+      <c r="D26" s="65"/>
+      <c r="E26" s="65"/>
+      <c r="F26" s="65"/>
+      <c r="G26" s="65"/>
+      <c r="H26" s="65"/>
       <c r="I26" s="62"/>
       <c r="J26" s="61"/>
       <c r="K26" s="62"/>
@@ -2005,13 +2005,13 @@
       <c r="M26" s="50"/>
     </row>
     <row r="27" spans="1:13" s="32" customFormat="1" ht="15.75">
-      <c r="B27" s="74"/>
+      <c r="B27" s="110"/>
       <c r="C27" s="62"/>
-      <c r="D27" s="85"/>
-      <c r="E27" s="85"/>
-      <c r="F27" s="85"/>
-      <c r="G27" s="85"/>
-      <c r="H27" s="85"/>
+      <c r="D27" s="65"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="65"/>
+      <c r="G27" s="65"/>
+      <c r="H27" s="65"/>
       <c r="I27" s="62"/>
       <c r="J27" s="61"/>
       <c r="K27" s="62"/>
@@ -2019,13 +2019,13 @@
       <c r="M27" s="34"/>
     </row>
     <row r="28" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B28" s="74"/>
+      <c r="B28" s="110"/>
       <c r="C28" s="62"/>
-      <c r="D28" s="82"/>
-      <c r="E28" s="83"/>
-      <c r="F28" s="83"/>
-      <c r="G28" s="83"/>
-      <c r="H28" s="84"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="74"/>
       <c r="I28" s="62"/>
       <c r="J28" s="61"/>
       <c r="K28" s="61"/>
@@ -2033,13 +2033,13 @@
       <c r="M28" s="48"/>
     </row>
     <row r="29" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B29" s="74"/>
+      <c r="B29" s="110"/>
       <c r="C29" s="62"/>
-      <c r="D29" s="85"/>
-      <c r="E29" s="85"/>
-      <c r="F29" s="85"/>
-      <c r="G29" s="85"/>
-      <c r="H29" s="85"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+      <c r="H29" s="65"/>
       <c r="I29" s="62"/>
       <c r="J29" s="61"/>
       <c r="K29" s="61"/>
@@ -2047,15 +2047,15 @@
       <c r="M29" s="49"/>
     </row>
     <row r="30" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B30" s="74"/>
+      <c r="B30" s="110"/>
       <c r="C30" s="62"/>
-      <c r="D30" s="129" t="s">
+      <c r="D30" s="75" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="130"/>
-      <c r="F30" s="130"/>
-      <c r="G30" s="130"/>
-      <c r="H30" s="131"/>
+      <c r="E30" s="76"/>
+      <c r="F30" s="76"/>
+      <c r="G30" s="76"/>
+      <c r="H30" s="77"/>
       <c r="I30" s="62"/>
       <c r="J30" s="61"/>
       <c r="K30" s="61"/>
@@ -2063,17 +2063,17 @@
       <c r="M30" s="43"/>
     </row>
     <row r="31" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B31" s="74"/>
+      <c r="B31" s="110"/>
       <c r="C31" s="62"/>
-      <c r="D31" s="85" t="s">
+      <c r="D31" s="65" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="65"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="62" t="s">
         <v>39</v>
-      </c>
-      <c r="E31" s="85"/>
-      <c r="F31" s="85"/>
-      <c r="G31" s="85"/>
-      <c r="H31" s="85"/>
-      <c r="I31" s="62" t="s">
-        <v>40</v>
       </c>
       <c r="J31" s="61"/>
       <c r="K31" s="41"/>
@@ -2081,13 +2081,13 @@
       <c r="M31" s="60"/>
     </row>
     <row r="32" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B32" s="74"/>
+      <c r="B32" s="110"/>
       <c r="C32" s="62"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="85"/>
-      <c r="F32" s="85"/>
-      <c r="G32" s="85"/>
-      <c r="H32" s="85"/>
+      <c r="D32" s="65"/>
+      <c r="E32" s="65"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="65"/>
+      <c r="H32" s="65"/>
       <c r="I32" s="62"/>
       <c r="J32" s="61"/>
       <c r="K32" s="61"/>
@@ -2095,13 +2095,13 @@
       <c r="M32" s="60"/>
     </row>
     <row r="33" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B33" s="74"/>
+      <c r="B33" s="110"/>
       <c r="C33" s="62"/>
-      <c r="D33" s="85"/>
-      <c r="E33" s="85"/>
-      <c r="F33" s="85"/>
-      <c r="G33" s="85"/>
-      <c r="H33" s="85"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
       <c r="I33" s="62"/>
       <c r="J33" s="61"/>
       <c r="K33" s="61"/>
@@ -2109,13 +2109,13 @@
       <c r="M33" s="47"/>
     </row>
     <row r="34" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B34" s="74"/>
+      <c r="B34" s="110"/>
       <c r="C34" s="62"/>
-      <c r="D34" s="85"/>
-      <c r="E34" s="85"/>
-      <c r="F34" s="85"/>
-      <c r="G34" s="85"/>
-      <c r="H34" s="85"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
       <c r="I34" s="62"/>
       <c r="J34" s="61"/>
       <c r="K34" s="61"/>
@@ -2123,13 +2123,13 @@
       <c r="M34" s="45"/>
     </row>
     <row r="35" spans="2:13" s="23" customFormat="1" ht="15.75">
-      <c r="B35" s="74"/>
+      <c r="B35" s="110"/>
       <c r="C35" s="62"/>
-      <c r="D35" s="85"/>
-      <c r="E35" s="85"/>
-      <c r="F35" s="85"/>
-      <c r="G35" s="85"/>
-      <c r="H35" s="85"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="65"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
       <c r="I35" s="62"/>
       <c r="J35" s="61"/>
       <c r="K35" s="61"/>
@@ -2137,13 +2137,13 @@
       <c r="M35" s="28"/>
     </row>
     <row r="36" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B36" s="74"/>
+      <c r="B36" s="110"/>
       <c r="C36" s="62"/>
-      <c r="D36" s="76"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="78"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="67"/>
+      <c r="G36" s="67"/>
+      <c r="H36" s="68"/>
       <c r="I36" s="62"/>
       <c r="J36" s="61"/>
       <c r="K36" s="61"/>
@@ -2151,13 +2151,13 @@
       <c r="M36" s="64"/>
     </row>
     <row r="37" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B37" s="74"/>
+      <c r="B37" s="110"/>
       <c r="C37" s="62"/>
-      <c r="D37" s="85"/>
-      <c r="E37" s="85"/>
-      <c r="F37" s="85"/>
-      <c r="G37" s="85"/>
-      <c r="H37" s="85"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
       <c r="I37" s="62"/>
       <c r="J37" s="61"/>
       <c r="K37" s="61"/>
@@ -2165,13 +2165,13 @@
       <c r="M37" s="58"/>
     </row>
     <row r="38" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B38" s="74"/>
+      <c r="B38" s="110"/>
       <c r="C38" s="62"/>
-      <c r="D38" s="85"/>
-      <c r="E38" s="85"/>
-      <c r="F38" s="85"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="85"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
+      <c r="H38" s="65"/>
       <c r="I38" s="62"/>
       <c r="J38" s="61"/>
       <c r="K38" s="61"/>
@@ -2179,13 +2179,13 @@
       <c r="M38" s="48"/>
     </row>
     <row r="39" spans="2:13" s="32" customFormat="1" ht="15.75">
-      <c r="B39" s="74"/>
+      <c r="B39" s="110"/>
       <c r="C39" s="42"/>
-      <c r="D39" s="85"/>
-      <c r="E39" s="85"/>
-      <c r="F39" s="85"/>
-      <c r="G39" s="85"/>
-      <c r="H39" s="85"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="65"/>
+      <c r="F39" s="65"/>
+      <c r="G39" s="65"/>
+      <c r="H39" s="65"/>
       <c r="I39" s="42"/>
       <c r="J39" s="41"/>
       <c r="K39" s="41"/>
@@ -2193,13 +2193,13 @@
       <c r="M39" s="34"/>
     </row>
     <row r="40" spans="2:13" s="23" customFormat="1" ht="15.75">
-      <c r="B40" s="74"/>
+      <c r="B40" s="110"/>
       <c r="C40" s="42"/>
-      <c r="D40" s="82"/>
-      <c r="E40" s="83"/>
-      <c r="F40" s="83"/>
-      <c r="G40" s="83"/>
-      <c r="H40" s="84"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="74"/>
       <c r="I40" s="42"/>
       <c r="J40" s="41"/>
       <c r="K40" s="41"/>
@@ -2207,13 +2207,13 @@
       <c r="M40" s="31"/>
     </row>
     <row r="41" spans="2:13" s="32" customFormat="1" ht="15.75">
-      <c r="B41" s="74"/>
+      <c r="B41" s="110"/>
       <c r="C41" s="42"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="83"/>
-      <c r="F41" s="83"/>
-      <c r="G41" s="83"/>
-      <c r="H41" s="84"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="74"/>
       <c r="I41" s="42"/>
       <c r="J41" s="41"/>
       <c r="K41" s="41"/>
@@ -2221,13 +2221,13 @@
       <c r="M41" s="33"/>
     </row>
     <row r="42" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B42" s="74"/>
+      <c r="B42" s="110"/>
       <c r="C42" s="42"/>
-      <c r="D42" s="85"/>
-      <c r="E42" s="85"/>
-      <c r="F42" s="85"/>
-      <c r="G42" s="85"/>
-      <c r="H42" s="85"/>
+      <c r="D42" s="65"/>
+      <c r="E42" s="65"/>
+      <c r="F42" s="65"/>
+      <c r="G42" s="65"/>
+      <c r="H42" s="65"/>
       <c r="I42" s="42"/>
       <c r="J42" s="41"/>
       <c r="K42" s="41"/>
@@ -2235,13 +2235,13 @@
       <c r="M42" s="48"/>
     </row>
     <row r="43" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B43" s="74"/>
+      <c r="B43" s="110"/>
       <c r="C43" s="42"/>
-      <c r="D43" s="85"/>
-      <c r="E43" s="85"/>
-      <c r="F43" s="85"/>
-      <c r="G43" s="85"/>
-      <c r="H43" s="85"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="65"/>
+      <c r="F43" s="65"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="65"/>
       <c r="I43" s="42"/>
       <c r="J43" s="41"/>
       <c r="K43" s="41"/>
@@ -2249,13 +2249,13 @@
       <c r="M43" s="44"/>
     </row>
     <row r="44" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B44" s="74"/>
+      <c r="B44" s="110"/>
       <c r="C44" s="42"/>
-      <c r="D44" s="76"/>
-      <c r="E44" s="77"/>
-      <c r="F44" s="77"/>
-      <c r="G44" s="77"/>
-      <c r="H44" s="78"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="68"/>
       <c r="I44" s="42"/>
       <c r="J44" s="41"/>
       <c r="K44" s="41"/>
@@ -2263,13 +2263,13 @@
       <c r="M44" s="54"/>
     </row>
     <row r="45" spans="2:13" s="23" customFormat="1" ht="15.75">
-      <c r="B45" s="74"/>
+      <c r="B45" s="110"/>
       <c r="C45" s="42"/>
-      <c r="D45" s="85"/>
-      <c r="E45" s="85"/>
-      <c r="F45" s="85"/>
-      <c r="G45" s="85"/>
-      <c r="H45" s="85"/>
+      <c r="D45" s="65"/>
+      <c r="E45" s="65"/>
+      <c r="F45" s="65"/>
+      <c r="G45" s="65"/>
+      <c r="H45" s="65"/>
       <c r="I45" s="42"/>
       <c r="J45" s="41"/>
       <c r="K45" s="41"/>
@@ -2277,15 +2277,15 @@
       <c r="M45" s="30"/>
     </row>
     <row r="46" spans="2:13" s="23" customFormat="1" ht="15.75">
-      <c r="B46" s="74"/>
+      <c r="B46" s="110"/>
       <c r="C46" s="42"/>
-      <c r="D46" s="129" t="s">
-        <v>43</v>
-      </c>
-      <c r="E46" s="130"/>
-      <c r="F46" s="130"/>
-      <c r="G46" s="130"/>
-      <c r="H46" s="131"/>
+      <c r="D46" s="75" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="76"/>
+      <c r="F46" s="76"/>
+      <c r="G46" s="76"/>
+      <c r="H46" s="77"/>
       <c r="I46" s="42"/>
       <c r="J46" s="41"/>
       <c r="K46" s="41"/>
@@ -2293,15 +2293,15 @@
       <c r="M46" s="29"/>
     </row>
     <row r="47" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B47" s="74"/>
+      <c r="B47" s="110"/>
       <c r="C47" s="42"/>
-      <c r="D47" s="76" t="s">
-        <v>46</v>
-      </c>
-      <c r="E47" s="77"/>
-      <c r="F47" s="77"/>
-      <c r="G47" s="77"/>
-      <c r="H47" s="78"/>
+      <c r="D47" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" s="67"/>
+      <c r="F47" s="67"/>
+      <c r="G47" s="67"/>
+      <c r="H47" s="68"/>
       <c r="I47" s="42"/>
       <c r="J47" s="41"/>
       <c r="K47" s="41"/>
@@ -2309,15 +2309,15 @@
       <c r="M47" s="46"/>
     </row>
     <row r="48" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B48" s="74"/>
+      <c r="B48" s="110"/>
       <c r="C48" s="42"/>
-      <c r="D48" s="76" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="77"/>
-      <c r="F48" s="77"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="78"/>
+      <c r="D48" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="67"/>
+      <c r="F48" s="67"/>
+      <c r="G48" s="67"/>
+      <c r="H48" s="68"/>
       <c r="I48" s="42"/>
       <c r="J48" s="41"/>
       <c r="K48" s="41"/>
@@ -2325,15 +2325,15 @@
       <c r="M48" s="51"/>
     </row>
     <row r="49" spans="2:15" s="40" customFormat="1" ht="15.75">
-      <c r="B49" s="74"/>
+      <c r="B49" s="110"/>
       <c r="C49" s="42"/>
-      <c r="D49" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="E49" s="77"/>
-      <c r="F49" s="77"/>
-      <c r="G49" s="77"/>
-      <c r="H49" s="78"/>
+      <c r="D49" s="66" t="s">
+        <v>42</v>
+      </c>
+      <c r="E49" s="67"/>
+      <c r="F49" s="67"/>
+      <c r="G49" s="67"/>
+      <c r="H49" s="68"/>
       <c r="I49" s="42"/>
       <c r="J49" s="41"/>
       <c r="K49" s="41"/>
@@ -2341,15 +2341,15 @@
       <c r="M49" s="51"/>
     </row>
     <row r="50" spans="2:15" s="40" customFormat="1" ht="15.75">
-      <c r="B50" s="74"/>
+      <c r="B50" s="110"/>
       <c r="C50" s="42"/>
-      <c r="D50" s="129" t="s">
+      <c r="D50" s="75" t="s">
         <v>2</v>
       </c>
-      <c r="E50" s="130"/>
-      <c r="F50" s="130"/>
-      <c r="G50" s="130"/>
-      <c r="H50" s="131"/>
+      <c r="E50" s="76"/>
+      <c r="F50" s="76"/>
+      <c r="G50" s="76"/>
+      <c r="H50" s="77"/>
       <c r="I50" s="42"/>
       <c r="J50" s="41"/>
       <c r="K50" s="41"/>
@@ -2357,15 +2357,15 @@
       <c r="M50" s="57"/>
     </row>
     <row r="51" spans="2:15" s="32" customFormat="1" ht="15.75">
-      <c r="B51" s="74"/>
+      <c r="B51" s="110"/>
       <c r="C51" s="42"/>
-      <c r="D51" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="E51" s="77"/>
-      <c r="F51" s="77"/>
-      <c r="G51" s="77"/>
-      <c r="H51" s="78"/>
+      <c r="D51" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" s="67"/>
+      <c r="F51" s="67"/>
+      <c r="G51" s="67"/>
+      <c r="H51" s="68"/>
       <c r="I51" s="42"/>
       <c r="J51" s="41"/>
       <c r="K51" s="41"/>
@@ -2373,15 +2373,15 @@
       <c r="M51" s="37"/>
     </row>
     <row r="52" spans="2:15" s="32" customFormat="1" ht="15.75">
-      <c r="B52" s="74"/>
+      <c r="B52" s="110"/>
       <c r="C52" s="39"/>
-      <c r="D52" s="76" t="s">
-        <v>47</v>
-      </c>
-      <c r="E52" s="77"/>
-      <c r="F52" s="77"/>
-      <c r="G52" s="77"/>
-      <c r="H52" s="78"/>
+      <c r="D52" s="66" t="s">
+        <v>45</v>
+      </c>
+      <c r="E52" s="67"/>
+      <c r="F52" s="67"/>
+      <c r="G52" s="67"/>
+      <c r="H52" s="68"/>
       <c r="I52" s="39"/>
       <c r="J52" s="38"/>
       <c r="K52" s="38"/>
@@ -2389,13 +2389,13 @@
       <c r="M52" s="37"/>
     </row>
     <row r="53" spans="2:15" ht="15.75">
-      <c r="B53" s="74"/>
+      <c r="B53" s="110"/>
       <c r="C53" s="16"/>
-      <c r="D53" s="76"/>
-      <c r="E53" s="77"/>
-      <c r="F53" s="77"/>
-      <c r="G53" s="77"/>
-      <c r="H53" s="78"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="67"/>
+      <c r="F53" s="67"/>
+      <c r="G53" s="67"/>
+      <c r="H53" s="68"/>
       <c r="I53" s="16"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -2405,191 +2405,191 @@
       <c r="O53" s="9"/>
     </row>
     <row r="54" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B54" s="74"/>
-      <c r="C54" s="123" t="s">
+      <c r="B54" s="110"/>
+      <c r="C54" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="D54" s="124"/>
-      <c r="E54" s="124"/>
-      <c r="F54" s="124"/>
-      <c r="G54" s="124"/>
-      <c r="H54" s="124"/>
-      <c r="I54" s="124"/>
-      <c r="J54" s="124"/>
-      <c r="K54" s="124"/>
-      <c r="L54" s="125"/>
+      <c r="D54" s="91"/>
+      <c r="E54" s="91"/>
+      <c r="F54" s="91"/>
+      <c r="G54" s="91"/>
+      <c r="H54" s="91"/>
+      <c r="I54" s="91"/>
+      <c r="J54" s="91"/>
+      <c r="K54" s="91"/>
+      <c r="L54" s="92"/>
       <c r="M54" s="19"/>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
     </row>
     <row r="55" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B55" s="74"/>
-      <c r="C55" s="126"/>
-      <c r="D55" s="127"/>
-      <c r="E55" s="127"/>
-      <c r="F55" s="127"/>
-      <c r="G55" s="127"/>
-      <c r="H55" s="127"/>
-      <c r="I55" s="127"/>
-      <c r="J55" s="127"/>
-      <c r="K55" s="127"/>
-      <c r="L55" s="128"/>
+      <c r="B55" s="110"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="94"/>
+      <c r="E55" s="94"/>
+      <c r="F55" s="94"/>
+      <c r="G55" s="94"/>
+      <c r="H55" s="94"/>
+      <c r="I55" s="94"/>
+      <c r="J55" s="94"/>
+      <c r="K55" s="94"/>
+      <c r="L55" s="95"/>
       <c r="M55" s="19"/>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="2:15" ht="15" customHeight="1">
-      <c r="B56" s="74"/>
-      <c r="C56" s="114" t="s">
+      <c r="B56" s="110"/>
+      <c r="C56" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="D56" s="115"/>
-      <c r="E56" s="115"/>
-      <c r="F56" s="115"/>
-      <c r="G56" s="115"/>
-      <c r="H56" s="115"/>
-      <c r="I56" s="115"/>
-      <c r="J56" s="116"/>
-      <c r="K56" s="132" t="s">
-        <v>38</v>
-      </c>
-      <c r="L56" s="133"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="79"/>
+      <c r="F56" s="79"/>
+      <c r="G56" s="79"/>
+      <c r="H56" s="79"/>
+      <c r="I56" s="79"/>
+      <c r="J56" s="80"/>
+      <c r="K56" s="97" t="s">
+        <v>52</v>
+      </c>
+      <c r="L56" s="98"/>
       <c r="M56" s="19"/>
     </row>
     <row r="57" spans="2:15" ht="9" customHeight="1">
-      <c r="B57" s="74"/>
-      <c r="C57" s="117"/>
-      <c r="D57" s="118"/>
-      <c r="E57" s="118"/>
-      <c r="F57" s="118"/>
-      <c r="G57" s="118"/>
-      <c r="H57" s="118"/>
-      <c r="I57" s="118"/>
-      <c r="J57" s="119"/>
-      <c r="K57" s="134"/>
-      <c r="L57" s="135"/>
+      <c r="B57" s="110"/>
+      <c r="C57" s="81"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="82"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="82"/>
+      <c r="I57" s="82"/>
+      <c r="J57" s="83"/>
+      <c r="K57" s="99"/>
+      <c r="L57" s="100"/>
       <c r="M57" s="19"/>
     </row>
     <row r="58" spans="2:15" ht="3.75" customHeight="1">
-      <c r="B58" s="74"/>
-      <c r="C58" s="80"/>
-      <c r="D58" s="80"/>
-      <c r="E58" s="80"/>
-      <c r="F58" s="80"/>
-      <c r="G58" s="80"/>
-      <c r="H58" s="80"/>
-      <c r="I58" s="80"/>
-      <c r="J58" s="80"/>
-      <c r="K58" s="80"/>
-      <c r="L58" s="80"/>
+      <c r="B58" s="110"/>
+      <c r="C58" s="96"/>
+      <c r="D58" s="96"/>
+      <c r="E58" s="96"/>
+      <c r="F58" s="96"/>
+      <c r="G58" s="96"/>
+      <c r="H58" s="96"/>
+      <c r="I58" s="96"/>
+      <c r="J58" s="96"/>
+      <c r="K58" s="96"/>
+      <c r="L58" s="96"/>
       <c r="M58" s="19"/>
     </row>
     <row r="59" spans="2:15">
-      <c r="B59" s="74"/>
-      <c r="C59" s="120" t="s">
+      <c r="B59" s="110"/>
+      <c r="C59" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="D59" s="121"/>
-      <c r="E59" s="121"/>
-      <c r="F59" s="121"/>
-      <c r="G59" s="121"/>
-      <c r="H59" s="121"/>
-      <c r="I59" s="122"/>
-      <c r="J59" s="107" t="s">
+      <c r="D59" s="85"/>
+      <c r="E59" s="85"/>
+      <c r="F59" s="85"/>
+      <c r="G59" s="85"/>
+      <c r="H59" s="85"/>
+      <c r="I59" s="86"/>
+      <c r="J59" s="87" t="s">
         <v>10</v>
       </c>
-      <c r="K59" s="109"/>
-      <c r="L59" s="108"/>
+      <c r="K59" s="88"/>
+      <c r="L59" s="89"/>
       <c r="M59" s="19"/>
     </row>
     <row r="60" spans="2:15" ht="1.5" customHeight="1">
-      <c r="B60" s="74"/>
-      <c r="C60" s="111"/>
-      <c r="D60" s="112"/>
-      <c r="E60" s="112"/>
-      <c r="F60" s="112"/>
-      <c r="G60" s="112"/>
-      <c r="H60" s="112"/>
-      <c r="I60" s="113"/>
-      <c r="J60" s="92"/>
-      <c r="K60" s="93"/>
-      <c r="L60" s="94"/>
+      <c r="B60" s="110"/>
+      <c r="C60" s="113"/>
+      <c r="D60" s="114"/>
+      <c r="E60" s="114"/>
+      <c r="F60" s="114"/>
+      <c r="G60" s="114"/>
+      <c r="H60" s="114"/>
+      <c r="I60" s="115"/>
+      <c r="J60" s="104"/>
+      <c r="K60" s="105"/>
+      <c r="L60" s="106"/>
       <c r="M60" s="19"/>
     </row>
     <row r="61" spans="2:15" ht="3.75" customHeight="1">
-      <c r="B61" s="74"/>
-      <c r="C61" s="79"/>
-      <c r="D61" s="80"/>
-      <c r="E61" s="80"/>
-      <c r="F61" s="80"/>
-      <c r="G61" s="80"/>
-      <c r="H61" s="80"/>
-      <c r="I61" s="81"/>
-      <c r="J61" s="74"/>
-      <c r="K61" s="66"/>
-      <c r="L61" s="95"/>
+      <c r="B61" s="110"/>
+      <c r="C61" s="102"/>
+      <c r="D61" s="96"/>
+      <c r="E61" s="96"/>
+      <c r="F61" s="96"/>
+      <c r="G61" s="96"/>
+      <c r="H61" s="96"/>
+      <c r="I61" s="103"/>
+      <c r="J61" s="110"/>
+      <c r="K61" s="111"/>
+      <c r="L61" s="112"/>
       <c r="M61" s="19"/>
     </row>
     <row r="62" spans="2:15">
-      <c r="B62" s="74"/>
-      <c r="C62" s="107" t="s">
+      <c r="B62" s="110"/>
+      <c r="C62" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="108"/>
-      <c r="E62" s="107" t="s">
+      <c r="D62" s="89"/>
+      <c r="E62" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="F62" s="108"/>
-      <c r="G62" s="107" t="s">
+      <c r="F62" s="89"/>
+      <c r="G62" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="H62" s="109"/>
-      <c r="I62" s="108"/>
-      <c r="J62" s="74"/>
-      <c r="K62" s="66"/>
-      <c r="L62" s="95"/>
+      <c r="H62" s="88"/>
+      <c r="I62" s="89"/>
+      <c r="J62" s="110"/>
+      <c r="K62" s="111"/>
+      <c r="L62" s="112"/>
       <c r="M62" s="19"/>
     </row>
     <row r="63" spans="2:15">
-      <c r="B63" s="74"/>
-      <c r="C63" s="110"/>
-      <c r="D63" s="110"/>
-      <c r="E63" s="92"/>
-      <c r="F63" s="94"/>
-      <c r="G63" s="92"/>
-      <c r="H63" s="93"/>
-      <c r="I63" s="94"/>
-      <c r="J63" s="75"/>
-      <c r="K63" s="105"/>
-      <c r="L63" s="106"/>
+      <c r="B63" s="110"/>
+      <c r="C63" s="109"/>
+      <c r="D63" s="109"/>
+      <c r="E63" s="104"/>
+      <c r="F63" s="106"/>
+      <c r="G63" s="104"/>
+      <c r="H63" s="105"/>
+      <c r="I63" s="106"/>
+      <c r="J63" s="107"/>
+      <c r="K63" s="101"/>
+      <c r="L63" s="108"/>
       <c r="M63" s="19"/>
     </row>
     <row r="64" spans="2:15">
-      <c r="B64" s="74"/>
-      <c r="C64" s="110"/>
-      <c r="D64" s="110"/>
-      <c r="E64" s="75"/>
-      <c r="F64" s="106"/>
-      <c r="G64" s="75"/>
-      <c r="H64" s="105"/>
-      <c r="I64" s="106"/>
-      <c r="J64" s="79"/>
-      <c r="K64" s="80"/>
-      <c r="L64" s="81"/>
+      <c r="B64" s="110"/>
+      <c r="C64" s="109"/>
+      <c r="D64" s="109"/>
+      <c r="E64" s="107"/>
+      <c r="F64" s="108"/>
+      <c r="G64" s="107"/>
+      <c r="H64" s="101"/>
+      <c r="I64" s="108"/>
+      <c r="J64" s="102"/>
+      <c r="K64" s="96"/>
+      <c r="L64" s="103"/>
       <c r="M64" s="19"/>
     </row>
     <row r="65" spans="2:13" ht="6.75" customHeight="1">
-      <c r="B65" s="75"/>
-      <c r="C65" s="105"/>
-      <c r="D65" s="105"/>
-      <c r="E65" s="105"/>
-      <c r="F65" s="105"/>
-      <c r="G65" s="105"/>
-      <c r="H65" s="105"/>
-      <c r="I65" s="105"/>
-      <c r="J65" s="105"/>
-      <c r="K65" s="105"/>
-      <c r="L65" s="105"/>
+      <c r="B65" s="107"/>
+      <c r="C65" s="101"/>
+      <c r="D65" s="101"/>
+      <c r="E65" s="101"/>
+      <c r="F65" s="101"/>
+      <c r="G65" s="101"/>
+      <c r="H65" s="101"/>
+      <c r="I65" s="101"/>
+      <c r="J65" s="101"/>
+      <c r="K65" s="101"/>
+      <c r="L65" s="101"/>
       <c r="M65" s="18"/>
     </row>
     <row r="66" spans="2:13">
@@ -2608,62 +2608,6 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D36:H36"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D21:H21"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D26:H26"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="D19:H19"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="D20:H20"/>
-    <mergeCell ref="D22:H22"/>
-    <mergeCell ref="D48:H48"/>
-    <mergeCell ref="D40:H40"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D46:H46"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="D44:H44"/>
-    <mergeCell ref="C56:J57"/>
-    <mergeCell ref="C59:I59"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="J59:L59"/>
-    <mergeCell ref="D51:H51"/>
-    <mergeCell ref="C54:L55"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="K56:L57"/>
-    <mergeCell ref="C65:L65"/>
-    <mergeCell ref="J64:L64"/>
-    <mergeCell ref="G63:I64"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="E63:F64"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D64"/>
-    <mergeCell ref="J60:L63"/>
-    <mergeCell ref="C60:I60"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="M3:M9"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="B3:K4"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="C8:L9"/>
-    <mergeCell ref="F6:K6"/>
-    <mergeCell ref="F5:L5"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="D13:I13"/>
     <mergeCell ref="D15:H15"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="D16:H16"/>
@@ -2680,6 +2624,62 @@
     <mergeCell ref="D25:H25"/>
     <mergeCell ref="D27:H27"/>
     <mergeCell ref="D28:H28"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="M3:M9"/>
+    <mergeCell ref="F7:K7"/>
+    <mergeCell ref="B3:K4"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="C8:L9"/>
+    <mergeCell ref="F6:K6"/>
+    <mergeCell ref="F5:L5"/>
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="D13:I13"/>
+    <mergeCell ref="C65:L65"/>
+    <mergeCell ref="J64:L64"/>
+    <mergeCell ref="G63:I64"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="E63:F64"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D64"/>
+    <mergeCell ref="J60:L63"/>
+    <mergeCell ref="C60:I60"/>
+    <mergeCell ref="C56:J57"/>
+    <mergeCell ref="C59:I59"/>
+    <mergeCell ref="D49:H49"/>
+    <mergeCell ref="J59:L59"/>
+    <mergeCell ref="D51:H51"/>
+    <mergeCell ref="C54:L55"/>
+    <mergeCell ref="D50:H50"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="K56:L57"/>
+    <mergeCell ref="D48:H48"/>
+    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="D30:H30"/>
+    <mergeCell ref="D43:H43"/>
+    <mergeCell ref="D38:H38"/>
+    <mergeCell ref="D42:H42"/>
+    <mergeCell ref="D46:H46"/>
+    <mergeCell ref="D35:H35"/>
+    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="D29:H29"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D23:H23"/>
+    <mergeCell ref="D26:H26"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="D19:H19"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="D20:H20"/>
+    <mergeCell ref="D22:H22"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
fix height problem in generated excel
</commit_message>
<xml_diff>
--- a/src/main/resources/jxl_template.xlsx
+++ b/src/main/resources/jxl_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brookfield\IdeaProjects\fp\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822F2371-D793-48C0-919E-EE2BEC6F7963}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000C9000-00FD-4323-8621-C8C473D621DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -93,7 +93,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A31" authorId="0" shapeId="0" xr:uid="{D7EE34FC-B4ED-499D-820F-D65904C94320}">
+    <comment ref="A22" authorId="0" shapeId="0" xr:uid="{D7EE34FC-B4ED-499D-820F-D65904C94320}">
       <text>
         <r>
           <rPr>
@@ -113,7 +113,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="order.promo" var="promo" lastCell="M31")</t>
+jx:each(items="order.promo" var="promo" lastCell="M22")</t>
         </r>
       </text>
     </comment>
@@ -647,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -703,22 +703,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -777,37 +762,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -818,24 +794,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -997,6 +955,12 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1026,6 +990,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R66"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A42" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A18" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1556,169 +1523,169 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="8.25" customHeight="1">
-      <c r="B1" s="119"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="121"/>
+      <c r="B1" s="105"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="107"/>
     </row>
     <row r="2" spans="1:18" ht="4.5" customHeight="1">
-      <c r="B2" s="104"/>
-      <c r="C2" s="105"/>
-      <c r="D2" s="105"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="105"/>
-      <c r="M2" s="106"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="92"/>
       <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
-      <c r="K3" s="125"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="110"/>
+      <c r="E3" s="110"/>
+      <c r="F3" s="110"/>
+      <c r="G3" s="110"/>
+      <c r="H3" s="110"/>
+      <c r="I3" s="110"/>
+      <c r="J3" s="110"/>
+      <c r="K3" s="111"/>
       <c r="L3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="M3" s="112"/>
+      <c r="M3" s="98"/>
       <c r="O3" s="20"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="B4" s="123"/>
-      <c r="C4" s="124"/>
-      <c r="D4" s="124"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="124"/>
-      <c r="G4" s="124"/>
-      <c r="H4" s="124"/>
-      <c r="I4" s="124"/>
-      <c r="J4" s="124"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="36" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="111"/>
+      <c r="L4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="M4" s="112"/>
+      <c r="M4" s="98"/>
       <c r="O4" s="20"/>
     </row>
     <row r="5" spans="1:18" ht="15.75">
-      <c r="B5" s="110"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
       <c r="E5" s="11"/>
-      <c r="F5" s="122" t="s">
+      <c r="F5" s="108" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="122"/>
-      <c r="H5" s="122"/>
-      <c r="I5" s="122"/>
-      <c r="J5" s="122"/>
-      <c r="K5" s="122"/>
-      <c r="L5" s="122"/>
-      <c r="M5" s="112"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="98"/>
       <c r="O5" s="20"/>
     </row>
     <row r="6" spans="1:18" ht="15.75">
-      <c r="B6" s="110"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
       <c r="E6" s="11"/>
-      <c r="F6" s="122" t="s">
+      <c r="F6" s="108" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="122"/>
-      <c r="H6" s="122"/>
-      <c r="I6" s="122"/>
-      <c r="J6" s="122"/>
-      <c r="K6" s="128"/>
+      <c r="G6" s="108"/>
+      <c r="H6" s="108"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="114"/>
       <c r="L6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="M6" s="112"/>
+      <c r="M6" s="98"/>
       <c r="O6" s="20"/>
     </row>
     <row r="7" spans="1:18" ht="15.75">
-      <c r="B7" s="110"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="122" t="s">
+      <c r="F7" s="108" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="122"/>
-      <c r="H7" s="122"/>
-      <c r="I7" s="122"/>
-      <c r="J7" s="122"/>
-      <c r="K7" s="122"/>
-      <c r="L7" s="35" t="s">
+      <c r="G7" s="108"/>
+      <c r="H7" s="108"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="108"/>
+      <c r="K7" s="108"/>
+      <c r="L7" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="M7" s="112"/>
+      <c r="M7" s="98"/>
       <c r="O7" s="20"/>
       <c r="P7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1">
-      <c r="B8" s="110"/>
-      <c r="C8" s="126" t="s">
+      <c r="B8" s="96"/>
+      <c r="C8" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="127"/>
-      <c r="E8" s="127"/>
-      <c r="F8" s="127"/>
-      <c r="G8" s="127"/>
-      <c r="H8" s="127"/>
-      <c r="I8" s="127"/>
-      <c r="J8" s="127"/>
-      <c r="K8" s="127"/>
-      <c r="L8" s="127"/>
-      <c r="M8" s="112"/>
+      <c r="D8" s="113"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="113"/>
+      <c r="G8" s="113"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="113"/>
+      <c r="J8" s="113"/>
+      <c r="K8" s="113"/>
+      <c r="L8" s="113"/>
+      <c r="M8" s="98"/>
       <c r="O8" s="20"/>
     </row>
     <row r="9" spans="1:18" ht="16.5" customHeight="1">
-      <c r="B9" s="110"/>
-      <c r="C9" s="127"/>
-      <c r="D9" s="127"/>
-      <c r="E9" s="127"/>
-      <c r="F9" s="127"/>
-      <c r="G9" s="127"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="127"/>
-      <c r="J9" s="127"/>
-      <c r="K9" s="127"/>
-      <c r="L9" s="127"/>
-      <c r="M9" s="112"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="113"/>
+      <c r="M9" s="98"/>
       <c r="O9" s="20"/>
       <c r="P9" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1">
-      <c r="B10" s="110"/>
-      <c r="C10" s="116" t="s">
+      <c r="B10" s="96"/>
+      <c r="C10" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="135" t="s">
+      <c r="D10" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="135"/>
-      <c r="F10" s="135"/>
-      <c r="G10" s="135"/>
-      <c r="H10" s="135"/>
-      <c r="I10" s="136"/>
+      <c r="E10" s="123"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="123"/>
+      <c r="H10" s="123"/>
+      <c r="I10" s="124"/>
       <c r="J10" s="10"/>
       <c r="K10" s="5" t="s">
         <v>11</v>
@@ -1733,14 +1700,14 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1">
-      <c r="B11" s="110"/>
-      <c r="C11" s="117"/>
-      <c r="D11" s="137"/>
-      <c r="E11" s="137"/>
-      <c r="F11" s="137"/>
-      <c r="G11" s="137"/>
-      <c r="H11" s="137"/>
-      <c r="I11" s="138"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="125"/>
+      <c r="F11" s="125"/>
+      <c r="G11" s="125"/>
+      <c r="H11" s="125"/>
+      <c r="I11" s="126"/>
       <c r="J11" s="10"/>
       <c r="K11" s="2" t="s">
         <v>47</v>
@@ -1752,18 +1719,18 @@
       <c r="O11" s="20"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
-      <c r="B12" s="110"/>
-      <c r="C12" s="117" t="s">
+      <c r="B12" s="96"/>
+      <c r="C12" s="103" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="73" t="s">
+      <c r="D12" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="73"/>
-      <c r="I12" s="74"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="115"/>
+      <c r="I12" s="116"/>
       <c r="J12" s="10"/>
       <c r="K12" s="2" t="s">
         <v>48</v>
@@ -1775,14 +1742,14 @@
       <c r="O12" s="20"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1">
-      <c r="B13" s="110"/>
-      <c r="C13" s="118"/>
-      <c r="D13" s="129"/>
-      <c r="E13" s="129"/>
-      <c r="F13" s="129"/>
-      <c r="G13" s="129"/>
-      <c r="H13" s="129"/>
-      <c r="I13" s="130"/>
+      <c r="B13" s="96"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="118"/>
       <c r="J13" s="10"/>
       <c r="K13" s="8" t="s">
         <v>0</v>
@@ -1795,33 +1762,33 @@
       <c r="P13" s="14"/>
     </row>
     <row r="14" spans="1:18" ht="7.5" customHeight="1">
-      <c r="B14" s="110"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="111"/>
-      <c r="G14" s="111"/>
-      <c r="H14" s="111"/>
-      <c r="I14" s="111"/>
-      <c r="J14" s="111"/>
-      <c r="K14" s="111"/>
-      <c r="L14" s="111"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
       <c r="M14" s="19"/>
       <c r="O14" s="20"/>
       <c r="P14" s="12"/>
     </row>
     <row r="15" spans="1:18" ht="15.75">
-      <c r="B15" s="110"/>
+      <c r="B15" s="96"/>
       <c r="C15" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="131" t="s">
+      <c r="D15" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="131"/>
-      <c r="F15" s="131"/>
-      <c r="G15" s="131"/>
-      <c r="H15" s="131"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="119"/>
       <c r="I15" s="13" t="s">
         <v>4</v>
       </c>
@@ -1839,563 +1806,513 @@
       <c r="R15" s="27"/>
     </row>
     <row r="16" spans="1:18" s="20" customFormat="1" ht="15.75">
-      <c r="B16" s="110"/>
+      <c r="B16" s="96"/>
       <c r="C16" s="24"/>
-      <c r="D16" s="132"/>
-      <c r="E16" s="133"/>
-      <c r="F16" s="133"/>
-      <c r="G16" s="133"/>
-      <c r="H16" s="134"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="121"/>
+      <c r="F16" s="121"/>
+      <c r="G16" s="121"/>
+      <c r="H16" s="122"/>
       <c r="I16" s="21"/>
       <c r="J16" s="21"/>
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="22"/>
     </row>
-    <row r="17" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B17" s="110"/>
+    <row r="17" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B17" s="96"/>
       <c r="C17" s="25"/>
-      <c r="D17" s="69" t="s">
+      <c r="D17" s="55" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="70"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="70"/>
-      <c r="H17" s="71"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="57"/>
       <c r="I17" s="21"/>
       <c r="J17" s="21"/>
       <c r="K17" s="21"/>
       <c r="L17" s="21"/>
-      <c r="M17" s="63"/>
-    </row>
-    <row r="18" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B18" s="110"/>
-      <c r="C18" s="62"/>
-      <c r="D18" s="65" t="s">
+      <c r="M17" s="52"/>
+    </row>
+    <row r="18" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B18" s="96"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="62" t="s">
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="61" t="s">
+      <c r="J18" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="K18" s="62" t="s">
+      <c r="K18" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="61" t="s">
+      <c r="L18" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="M18" s="55"/>
-    </row>
-    <row r="19" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B19" s="110"/>
-      <c r="C19" s="62"/>
-      <c r="D19" s="65"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="65"/>
-      <c r="H19" s="65"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="62"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="47"/>
-    </row>
-    <row r="20" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B20" s="110"/>
-      <c r="C20" s="62"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="56"/>
-    </row>
-    <row r="21" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B21" s="110"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="61"/>
-      <c r="K21" s="62"/>
-      <c r="L21" s="61"/>
-      <c r="M21" s="63"/>
-    </row>
-    <row r="22" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B22" s="110"/>
-      <c r="C22" s="62"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="62"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="59"/>
-    </row>
-    <row r="23" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B23" s="110"/>
-      <c r="C23" s="62"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="65"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="53"/>
-    </row>
-    <row r="24" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B24" s="110"/>
-      <c r="C24" s="62"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="G24" s="65"/>
-      <c r="H24" s="65"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="62"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="52"/>
-    </row>
-    <row r="25" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B25" s="110"/>
-      <c r="C25" s="62"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="62"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="47"/>
-    </row>
-    <row r="26" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B26" s="110"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="65"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="65"/>
-      <c r="G26" s="65"/>
-      <c r="H26" s="65"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="50"/>
-    </row>
-    <row r="27" spans="1:13" s="32" customFormat="1" ht="15.75">
-      <c r="B27" s="110"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="65"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="65"/>
-      <c r="G27" s="65"/>
-      <c r="H27" s="65"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="34"/>
-    </row>
-    <row r="28" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B28" s="110"/>
-      <c r="C28" s="62"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="73"/>
-      <c r="F28" s="73"/>
-      <c r="G28" s="73"/>
-      <c r="H28" s="74"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="48"/>
-    </row>
-    <row r="29" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B29" s="110"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="65"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="49"/>
-    </row>
-    <row r="30" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B30" s="110"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="75" t="s">
+      <c r="M18" s="46"/>
+    </row>
+    <row r="19" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B19" s="96"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="41"/>
+    </row>
+    <row r="20" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B20" s="96"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="54"/>
+      <c r="H20" s="54"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="47"/>
+    </row>
+    <row r="21" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B21" s="96"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="77"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="43"/>
-    </row>
-    <row r="31" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B31" s="110"/>
-      <c r="C31" s="62"/>
-      <c r="D31" s="65" t="s">
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="63"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="50"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="38"/>
+    </row>
+    <row r="22" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B22" s="96"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="54" t="s">
         <v>38</v>
       </c>
-      <c r="E31" s="65"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="65"/>
-      <c r="H31" s="65"/>
-      <c r="I31" s="62" t="s">
+      <c r="E22" s="54"/>
+      <c r="F22" s="54"/>
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="51" t="s">
         <v>39</v>
       </c>
-      <c r="J31" s="61"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="60"/>
-    </row>
-    <row r="32" spans="1:13" s="40" customFormat="1" ht="15.75">
-      <c r="B32" s="110"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="65"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="65"/>
-      <c r="G32" s="65"/>
-      <c r="H32" s="65"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="60"/>
-    </row>
-    <row r="33" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B33" s="110"/>
-      <c r="C33" s="62"/>
-      <c r="D33" s="65"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="65"/>
-      <c r="G33" s="65"/>
-      <c r="H33" s="65"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="47"/>
-    </row>
-    <row r="34" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B34" s="110"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="65"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="65"/>
-      <c r="G34" s="65"/>
-      <c r="H34" s="65"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="61"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="45"/>
-    </row>
-    <row r="35" spans="2:13" s="23" customFormat="1" ht="15.75">
-      <c r="B35" s="110"/>
-      <c r="C35" s="62"/>
-      <c r="D35" s="65"/>
-      <c r="E35" s="65"/>
-      <c r="F35" s="65"/>
-      <c r="G35" s="65"/>
-      <c r="H35" s="65"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="61"/>
-      <c r="K35" s="61"/>
-      <c r="L35" s="61"/>
-      <c r="M35" s="28"/>
-    </row>
-    <row r="36" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B36" s="110"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="62"/>
-      <c r="J36" s="61"/>
-      <c r="K36" s="61"/>
-      <c r="L36" s="61"/>
-      <c r="M36" s="64"/>
-    </row>
-    <row r="37" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B37" s="110"/>
-      <c r="C37" s="62"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="49"/>
+    </row>
+    <row r="23" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B23" s="96"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="54"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="54"/>
+      <c r="G23" s="54"/>
+      <c r="H23" s="54"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="45"/>
+    </row>
+    <row r="24" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B24" s="96"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="54"/>
+      <c r="E24" s="54"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="54"/>
+      <c r="H24" s="54"/>
+      <c r="I24" s="51"/>
+      <c r="J24" s="50"/>
+      <c r="K24" s="51"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="44"/>
+    </row>
+    <row r="25" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B25" s="96"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="M25" s="28"/>
+    </row>
+    <row r="26" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B26" s="96"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="58" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="60"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="40"/>
+    </row>
+    <row r="27" spans="1:13" s="29" customFormat="1" ht="15.75">
+      <c r="B27" s="96"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="43"/>
+    </row>
+    <row r="28" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B28" s="96"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="60"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
+      <c r="M28" s="43"/>
+    </row>
+    <row r="29" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B29" s="96"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="54"/>
+      <c r="E29" s="54"/>
+      <c r="F29" s="54"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="50"/>
+      <c r="K29" s="50"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="42"/>
+    </row>
+    <row r="30" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B30" s="96"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="61" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="63"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="36"/>
+      <c r="K30" s="36"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="48"/>
+    </row>
+    <row r="31" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B31" s="96"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="58" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" s="59"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="36"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="32"/>
+    </row>
+    <row r="32" spans="1:13" s="35" customFormat="1" ht="15.75">
+      <c r="B32" s="96"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="58" t="s">
+        <v>45</v>
+      </c>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="60"/>
+      <c r="I32" s="34"/>
+      <c r="J32" s="33"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="32"/>
+    </row>
+    <row r="33" spans="2:13" s="35" customFormat="1" ht="15.75">
+      <c r="B33" s="96"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="127"/>
+      <c r="E33" s="115"/>
+      <c r="F33" s="115"/>
+      <c r="G33" s="115"/>
+      <c r="H33" s="116"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="50"/>
+      <c r="K33" s="50"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="53"/>
+    </row>
+    <row r="34" spans="2:13" s="35" customFormat="1" ht="15.75">
+      <c r="B34" s="96"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="50"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="39"/>
+    </row>
+    <row r="35" spans="2:13" s="23" customFormat="1">
+      <c r="B35" s="96"/>
+      <c r="C35" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="77"/>
+      <c r="G35" s="77"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="77"/>
+      <c r="J35" s="77"/>
+      <c r="K35" s="77"/>
+      <c r="L35" s="78"/>
+      <c r="M35" s="19"/>
+    </row>
+    <row r="36" spans="2:13" s="35" customFormat="1">
+      <c r="B36" s="96"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="80"/>
+      <c r="F36" s="80"/>
+      <c r="G36" s="80"/>
+      <c r="H36" s="80"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="81"/>
+      <c r="M36" s="19"/>
+    </row>
+    <row r="37" spans="2:13" s="35" customFormat="1">
+      <c r="B37" s="96"/>
+      <c r="C37" s="64" t="s">
+        <v>17</v>
+      </c>
       <c r="D37" s="65"/>
       <c r="E37" s="65"/>
       <c r="F37" s="65"/>
       <c r="G37" s="65"/>
       <c r="H37" s="65"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="61"/>
-      <c r="L37" s="61"/>
-      <c r="M37" s="58"/>
-    </row>
-    <row r="38" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B38" s="110"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="65"/>
-      <c r="E38" s="65"/>
-      <c r="F38" s="65"/>
-      <c r="G38" s="65"/>
-      <c r="H38" s="65"/>
-      <c r="I38" s="62"/>
-      <c r="J38" s="61"/>
-      <c r="K38" s="61"/>
-      <c r="L38" s="61"/>
-      <c r="M38" s="48"/>
-    </row>
-    <row r="39" spans="2:13" s="32" customFormat="1" ht="15.75">
-      <c r="B39" s="110"/>
-      <c r="C39" s="42"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="65"/>
-      <c r="H39" s="65"/>
-      <c r="I39" s="42"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="41"/>
-      <c r="M39" s="34"/>
-    </row>
-    <row r="40" spans="2:13" s="23" customFormat="1" ht="15.75">
-      <c r="B40" s="110"/>
-      <c r="C40" s="42"/>
-      <c r="D40" s="72"/>
-      <c r="E40" s="73"/>
-      <c r="F40" s="73"/>
-      <c r="G40" s="73"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="42"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="41"/>
-      <c r="L40" s="41"/>
-      <c r="M40" s="31"/>
-    </row>
-    <row r="41" spans="2:13" s="32" customFormat="1" ht="15.75">
-      <c r="B41" s="110"/>
-      <c r="C41" s="42"/>
-      <c r="D41" s="72"/>
-      <c r="E41" s="73"/>
-      <c r="F41" s="73"/>
-      <c r="G41" s="73"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="41"/>
-      <c r="M41" s="33"/>
-    </row>
-    <row r="42" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B42" s="110"/>
-      <c r="C42" s="42"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="65"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="65"/>
-      <c r="H42" s="65"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="41"/>
-      <c r="L42" s="41"/>
-      <c r="M42" s="48"/>
-    </row>
-    <row r="43" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B43" s="110"/>
-      <c r="C43" s="42"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="65"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="65"/>
-      <c r="H43" s="65"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="41"/>
-      <c r="L43" s="41"/>
-      <c r="M43" s="44"/>
-    </row>
-    <row r="44" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B44" s="110"/>
-      <c r="C44" s="42"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="67"/>
-      <c r="F44" s="67"/>
-      <c r="G44" s="67"/>
-      <c r="H44" s="68"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="41"/>
-      <c r="L44" s="41"/>
-      <c r="M44" s="54"/>
-    </row>
-    <row r="45" spans="2:13" s="23" customFormat="1" ht="15.75">
-      <c r="B45" s="110"/>
-      <c r="C45" s="42"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="65"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="65"/>
-      <c r="H45" s="65"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="41"/>
-      <c r="M45" s="30"/>
-    </row>
-    <row r="46" spans="2:13" s="23" customFormat="1" ht="15.75">
-      <c r="B46" s="110"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="75" t="s">
-        <v>41</v>
-      </c>
-      <c r="E46" s="76"/>
-      <c r="F46" s="76"/>
-      <c r="G46" s="76"/>
-      <c r="H46" s="77"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41"/>
-      <c r="M46" s="29"/>
-    </row>
-    <row r="47" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B47" s="110"/>
-      <c r="C47" s="42"/>
-      <c r="D47" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="67"/>
-      <c r="F47" s="67"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="68"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41"/>
-      <c r="L47" s="41"/>
-      <c r="M47" s="46"/>
-    </row>
-    <row r="48" spans="2:13" s="40" customFormat="1" ht="15.75">
-      <c r="B48" s="110"/>
-      <c r="C48" s="42"/>
-      <c r="D48" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="E48" s="67"/>
-      <c r="F48" s="67"/>
-      <c r="G48" s="67"/>
-      <c r="H48" s="68"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="41"/>
-      <c r="L48" s="41"/>
-      <c r="M48" s="51"/>
-    </row>
-    <row r="49" spans="2:15" s="40" customFormat="1" ht="15.75">
-      <c r="B49" s="110"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="66" t="s">
-        <v>42</v>
-      </c>
-      <c r="E49" s="67"/>
-      <c r="F49" s="67"/>
-      <c r="G49" s="67"/>
-      <c r="H49" s="68"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="41"/>
-      <c r="K49" s="41"/>
-      <c r="L49" s="41"/>
-      <c r="M49" s="51"/>
-    </row>
-    <row r="50" spans="2:15" s="40" customFormat="1" ht="15.75">
-      <c r="B50" s="110"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="75" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="76"/>
-      <c r="F50" s="76"/>
-      <c r="G50" s="76"/>
-      <c r="H50" s="77"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="41"/>
-      <c r="K50" s="41"/>
-      <c r="L50" s="41"/>
-      <c r="M50" s="57"/>
-    </row>
-    <row r="51" spans="2:15" s="32" customFormat="1" ht="15.75">
-      <c r="B51" s="110"/>
-      <c r="C51" s="42"/>
-      <c r="D51" s="66" t="s">
-        <v>43</v>
-      </c>
-      <c r="E51" s="67"/>
-      <c r="F51" s="67"/>
-      <c r="G51" s="67"/>
-      <c r="H51" s="68"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="41"/>
-      <c r="L51" s="41"/>
-      <c r="M51" s="37"/>
-    </row>
-    <row r="52" spans="2:15" s="32" customFormat="1" ht="15.75">
-      <c r="B52" s="110"/>
-      <c r="C52" s="39"/>
-      <c r="D52" s="66" t="s">
-        <v>45</v>
-      </c>
-      <c r="E52" s="67"/>
-      <c r="F52" s="67"/>
-      <c r="G52" s="67"/>
-      <c r="H52" s="68"/>
-      <c r="I52" s="39"/>
-      <c r="J52" s="38"/>
-      <c r="K52" s="38"/>
-      <c r="L52" s="38"/>
-      <c r="M52" s="37"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="83" t="s">
+        <v>52</v>
+      </c>
+      <c r="L37" s="84"/>
+      <c r="M37" s="19"/>
+    </row>
+    <row r="38" spans="2:13" s="35" customFormat="1">
+      <c r="B38" s="96"/>
+      <c r="C38" s="67"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="68"/>
+      <c r="F38" s="68"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="69"/>
+      <c r="K38" s="85"/>
+      <c r="L38" s="86"/>
+      <c r="M38" s="19"/>
+    </row>
+    <row r="39" spans="2:13" s="29" customFormat="1">
+      <c r="B39" s="96"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="82"/>
+      <c r="G39" s="82"/>
+      <c r="H39" s="82"/>
+      <c r="I39" s="82"/>
+      <c r="J39" s="82"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="82"/>
+      <c r="M39" s="19"/>
+    </row>
+    <row r="40" spans="2:13" s="23" customFormat="1">
+      <c r="B40" s="96"/>
+      <c r="C40" s="70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="71"/>
+      <c r="E40" s="71"/>
+      <c r="F40" s="71"/>
+      <c r="G40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="K40" s="74"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="19"/>
+    </row>
+    <row r="41" spans="2:13" s="29" customFormat="1">
+      <c r="B41" s="96"/>
+      <c r="C41" s="99"/>
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="100"/>
+      <c r="H41" s="100"/>
+      <c r="I41" s="101"/>
+      <c r="J41" s="90"/>
+      <c r="K41" s="91"/>
+      <c r="L41" s="92"/>
+      <c r="M41" s="19"/>
+    </row>
+    <row r="42" spans="2:13" s="35" customFormat="1">
+      <c r="B42" s="96"/>
+      <c r="C42" s="88"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="82"/>
+      <c r="G42" s="82"/>
+      <c r="H42" s="82"/>
+      <c r="I42" s="89"/>
+      <c r="J42" s="96"/>
+      <c r="K42" s="97"/>
+      <c r="L42" s="98"/>
+      <c r="M42" s="19"/>
+    </row>
+    <row r="43" spans="2:13" s="35" customFormat="1">
+      <c r="B43" s="96"/>
+      <c r="C43" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" s="75"/>
+      <c r="E43" s="73" t="s">
+        <v>21</v>
+      </c>
+      <c r="F43" s="75"/>
+      <c r="G43" s="73" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="74"/>
+      <c r="I43" s="75"/>
+      <c r="J43" s="96"/>
+      <c r="K43" s="97"/>
+      <c r="L43" s="98"/>
+      <c r="M43" s="19"/>
+    </row>
+    <row r="44" spans="2:13" s="35" customFormat="1">
+      <c r="B44" s="96"/>
+      <c r="C44" s="95"/>
+      <c r="D44" s="95"/>
+      <c r="E44" s="90"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="90"/>
+      <c r="H44" s="91"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="87"/>
+      <c r="L44" s="94"/>
+      <c r="M44" s="19"/>
+    </row>
+    <row r="45" spans="2:13" s="23" customFormat="1">
+      <c r="B45" s="96"/>
+      <c r="C45" s="95"/>
+      <c r="D45" s="95"/>
+      <c r="E45" s="93"/>
+      <c r="F45" s="94"/>
+      <c r="G45" s="93"/>
+      <c r="H45" s="87"/>
+      <c r="I45" s="94"/>
+      <c r="J45" s="88"/>
+      <c r="K45" s="82"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="19"/>
+    </row>
+    <row r="46" spans="2:13" s="23" customFormat="1">
+      <c r="B46" s="96"/>
+      <c r="C46" s="87"/>
+      <c r="D46" s="87"/>
+      <c r="E46" s="87"/>
+      <c r="F46" s="87"/>
+      <c r="G46" s="87"/>
+      <c r="H46" s="87"/>
+      <c r="I46" s="87"/>
+      <c r="J46" s="87"/>
+      <c r="K46" s="87"/>
+      <c r="L46" s="87"/>
+      <c r="M46" s="18"/>
+    </row>
+    <row r="47" spans="2:13" s="35" customFormat="1">
+      <c r="B47" s="96"/>
+    </row>
+    <row r="48" spans="2:13" s="35" customFormat="1">
+      <c r="B48" s="96"/>
+    </row>
+    <row r="49" spans="2:15" s="35" customFormat="1">
+      <c r="B49" s="96"/>
+    </row>
+    <row r="50" spans="2:15" s="35" customFormat="1">
+      <c r="B50" s="96"/>
+    </row>
+    <row r="51" spans="2:15" s="29" customFormat="1">
+      <c r="B51" s="96"/>
+    </row>
+    <row r="52" spans="2:15" s="29" customFormat="1">
+      <c r="B52" s="96"/>
     </row>
     <row r="53" spans="2:15" ht="15.75">
-      <c r="B53" s="110"/>
+      <c r="B53" s="96"/>
       <c r="C53" s="16"/>
-      <c r="D53" s="66"/>
-      <c r="E53" s="67"/>
-      <c r="F53" s="67"/>
-      <c r="G53" s="67"/>
-      <c r="H53" s="68"/>
+      <c r="D53" s="58"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="60"/>
       <c r="I53" s="16"/>
       <c r="J53" s="15"/>
       <c r="K53" s="15"/>
@@ -2405,192 +2322,44 @@
       <c r="O53" s="9"/>
     </row>
     <row r="54" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B54" s="110"/>
-      <c r="C54" s="90" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="91"/>
-      <c r="E54" s="91"/>
-      <c r="F54" s="91"/>
-      <c r="G54" s="91"/>
-      <c r="H54" s="91"/>
-      <c r="I54" s="91"/>
-      <c r="J54" s="91"/>
-      <c r="K54" s="91"/>
-      <c r="L54" s="92"/>
-      <c r="M54" s="19"/>
+      <c r="B54" s="96"/>
       <c r="N54" s="9"/>
       <c r="O54" s="9"/>
     </row>
     <row r="55" spans="2:15" ht="15.75" customHeight="1">
-      <c r="B55" s="110"/>
-      <c r="C55" s="93"/>
-      <c r="D55" s="94"/>
-      <c r="E55" s="94"/>
-      <c r="F55" s="94"/>
-      <c r="G55" s="94"/>
-      <c r="H55" s="94"/>
-      <c r="I55" s="94"/>
-      <c r="J55" s="94"/>
-      <c r="K55" s="94"/>
-      <c r="L55" s="95"/>
-      <c r="M55" s="19"/>
+      <c r="B55" s="96"/>
       <c r="N55" s="9"/>
       <c r="O55" s="9"/>
     </row>
     <row r="56" spans="2:15" ht="15" customHeight="1">
-      <c r="B56" s="110"/>
-      <c r="C56" s="78" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="79"/>
-      <c r="E56" s="79"/>
-      <c r="F56" s="79"/>
-      <c r="G56" s="79"/>
-      <c r="H56" s="79"/>
-      <c r="I56" s="79"/>
-      <c r="J56" s="80"/>
-      <c r="K56" s="97" t="s">
-        <v>52</v>
-      </c>
-      <c r="L56" s="98"/>
-      <c r="M56" s="19"/>
+      <c r="B56" s="96"/>
     </row>
     <row r="57" spans="2:15" ht="9" customHeight="1">
-      <c r="B57" s="110"/>
-      <c r="C57" s="81"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="82"/>
-      <c r="F57" s="82"/>
-      <c r="G57" s="82"/>
-      <c r="H57" s="82"/>
-      <c r="I57" s="82"/>
-      <c r="J57" s="83"/>
-      <c r="K57" s="99"/>
-      <c r="L57" s="100"/>
-      <c r="M57" s="19"/>
+      <c r="B57" s="96"/>
     </row>
     <row r="58" spans="2:15" ht="3.75" customHeight="1">
-      <c r="B58" s="110"/>
-      <c r="C58" s="96"/>
-      <c r="D58" s="96"/>
-      <c r="E58" s="96"/>
-      <c r="F58" s="96"/>
-      <c r="G58" s="96"/>
-      <c r="H58" s="96"/>
-      <c r="I58" s="96"/>
-      <c r="J58" s="96"/>
-      <c r="K58" s="96"/>
-      <c r="L58" s="96"/>
-      <c r="M58" s="19"/>
+      <c r="B58" s="96"/>
     </row>
     <row r="59" spans="2:15">
-      <c r="B59" s="110"/>
-      <c r="C59" s="84" t="s">
-        <v>6</v>
-      </c>
-      <c r="D59" s="85"/>
-      <c r="E59" s="85"/>
-      <c r="F59" s="85"/>
-      <c r="G59" s="85"/>
-      <c r="H59" s="85"/>
-      <c r="I59" s="86"/>
-      <c r="J59" s="87" t="s">
-        <v>10</v>
-      </c>
-      <c r="K59" s="88"/>
-      <c r="L59" s="89"/>
-      <c r="M59" s="19"/>
+      <c r="B59" s="96"/>
     </row>
     <row r="60" spans="2:15" ht="1.5" customHeight="1">
-      <c r="B60" s="110"/>
-      <c r="C60" s="113"/>
-      <c r="D60" s="114"/>
-      <c r="E60" s="114"/>
-      <c r="F60" s="114"/>
-      <c r="G60" s="114"/>
-      <c r="H60" s="114"/>
-      <c r="I60" s="115"/>
-      <c r="J60" s="104"/>
-      <c r="K60" s="105"/>
-      <c r="L60" s="106"/>
-      <c r="M60" s="19"/>
+      <c r="B60" s="96"/>
     </row>
     <row r="61" spans="2:15" ht="3.75" customHeight="1">
-      <c r="B61" s="110"/>
-      <c r="C61" s="102"/>
-      <c r="D61" s="96"/>
-      <c r="E61" s="96"/>
-      <c r="F61" s="96"/>
-      <c r="G61" s="96"/>
-      <c r="H61" s="96"/>
-      <c r="I61" s="103"/>
-      <c r="J61" s="110"/>
-      <c r="K61" s="111"/>
-      <c r="L61" s="112"/>
-      <c r="M61" s="19"/>
+      <c r="B61" s="96"/>
     </row>
     <row r="62" spans="2:15">
-      <c r="B62" s="110"/>
-      <c r="C62" s="87" t="s">
-        <v>19</v>
-      </c>
-      <c r="D62" s="89"/>
-      <c r="E62" s="87" t="s">
-        <v>21</v>
-      </c>
-      <c r="F62" s="89"/>
-      <c r="G62" s="87" t="s">
-        <v>20</v>
-      </c>
-      <c r="H62" s="88"/>
-      <c r="I62" s="89"/>
-      <c r="J62" s="110"/>
-      <c r="K62" s="111"/>
-      <c r="L62" s="112"/>
-      <c r="M62" s="19"/>
+      <c r="B62" s="96"/>
     </row>
     <row r="63" spans="2:15">
-      <c r="B63" s="110"/>
-      <c r="C63" s="109"/>
-      <c r="D63" s="109"/>
-      <c r="E63" s="104"/>
-      <c r="F63" s="106"/>
-      <c r="G63" s="104"/>
-      <c r="H63" s="105"/>
-      <c r="I63" s="106"/>
-      <c r="J63" s="107"/>
-      <c r="K63" s="101"/>
-      <c r="L63" s="108"/>
-      <c r="M63" s="19"/>
+      <c r="B63" s="96"/>
     </row>
     <row r="64" spans="2:15">
-      <c r="B64" s="110"/>
-      <c r="C64" s="109"/>
-      <c r="D64" s="109"/>
-      <c r="E64" s="107"/>
-      <c r="F64" s="108"/>
-      <c r="G64" s="107"/>
-      <c r="H64" s="101"/>
-      <c r="I64" s="108"/>
-      <c r="J64" s="102"/>
-      <c r="K64" s="96"/>
-      <c r="L64" s="103"/>
-      <c r="M64" s="19"/>
+      <c r="B64" s="96"/>
     </row>
     <row r="65" spans="2:13" ht="6.75" customHeight="1">
-      <c r="B65" s="107"/>
-      <c r="C65" s="101"/>
-      <c r="D65" s="101"/>
-      <c r="E65" s="101"/>
-      <c r="F65" s="101"/>
-      <c r="G65" s="101"/>
-      <c r="H65" s="101"/>
-      <c r="I65" s="101"/>
-      <c r="J65" s="101"/>
-      <c r="K65" s="101"/>
-      <c r="L65" s="101"/>
-      <c r="M65" s="18"/>
+      <c r="B65" s="93"/>
     </row>
     <row r="66" spans="2:13">
       <c r="B66" s="1"/>
@@ -2607,23 +2376,17 @@
       <c r="M66" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="54">
     <mergeCell ref="D15:H15"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="D16:H16"/>
     <mergeCell ref="D10:I11"/>
     <mergeCell ref="B10:B65"/>
-    <mergeCell ref="D52:H52"/>
+    <mergeCell ref="D32:H32"/>
     <mergeCell ref="D53:H53"/>
-    <mergeCell ref="C61:I61"/>
-    <mergeCell ref="D41:H41"/>
-    <mergeCell ref="D45:H45"/>
-    <mergeCell ref="D39:H39"/>
-    <mergeCell ref="D47:H47"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="D26:H26"/>
     <mergeCell ref="D33:H33"/>
-    <mergeCell ref="D25:H25"/>
-    <mergeCell ref="D27:H27"/>
-    <mergeCell ref="D28:H28"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="B1:F1"/>
@@ -2637,49 +2400,37 @@
     <mergeCell ref="F5:L5"/>
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="D13:I13"/>
-    <mergeCell ref="C65:L65"/>
-    <mergeCell ref="J64:L64"/>
-    <mergeCell ref="G63:I64"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="E63:F64"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D64"/>
-    <mergeCell ref="J60:L63"/>
-    <mergeCell ref="C60:I60"/>
-    <mergeCell ref="C56:J57"/>
-    <mergeCell ref="C59:I59"/>
-    <mergeCell ref="D49:H49"/>
-    <mergeCell ref="J59:L59"/>
-    <mergeCell ref="D51:H51"/>
-    <mergeCell ref="C54:L55"/>
-    <mergeCell ref="D50:H50"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="K56:L57"/>
-    <mergeCell ref="D48:H48"/>
-    <mergeCell ref="D40:H40"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="G44:I45"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="E44:F45"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D45"/>
+    <mergeCell ref="J41:L44"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="D34:H34"/>
+    <mergeCell ref="C37:J38"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="D28:H28"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="D31:H31"/>
+    <mergeCell ref="C35:L36"/>
     <mergeCell ref="D30:H30"/>
-    <mergeCell ref="D43:H43"/>
-    <mergeCell ref="D38:H38"/>
-    <mergeCell ref="D42:H42"/>
-    <mergeCell ref="D46:H46"/>
-    <mergeCell ref="D35:H35"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="D34:H34"/>
-    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="C39:L39"/>
+    <mergeCell ref="K37:L38"/>
     <mergeCell ref="D29:H29"/>
-    <mergeCell ref="D31:H31"/>
-    <mergeCell ref="D32:H32"/>
-    <mergeCell ref="D36:H36"/>
+    <mergeCell ref="D22:H22"/>
     <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D21:H21"/>
     <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D26:H26"/>
     <mergeCell ref="D24:H24"/>
     <mergeCell ref="D19:H19"/>
     <mergeCell ref="D18:H18"/>
     <mergeCell ref="D20:H20"/>
-    <mergeCell ref="D22:H22"/>
+    <mergeCell ref="D27:H27"/>
+    <mergeCell ref="D21:H21"/>
+    <mergeCell ref="D25:H25"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>